<commit_message>
refactor(grading): Make rarity bonus more conservative
- Changed from tiered bonuses (1/2/3) to flat +1 point
- Only award bonus for criteria with ≤15% prevalence (was ≤25%)
- Results in more balanced grade distribution
- Top score: 100 (1 student, was 3 students)
- Max bonus: +14 points (was +55 points)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/outputs/grades.xlsx
+++ b/outputs/grades.xlsx
@@ -520,26 +520,26 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>38950</t>
+          <t>38970</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
-        <v>84.21091445427729</v>
+        <v>90.56047197640117</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>100</v>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>35/58</t>
+          <t>41/58</t>
         </is>
       </c>
       <c r="G2" s="4" t="inlineStr">
         <is>
-          <t>E2E Tests (+3), Integration Tests (+3), Quick Start Guide (+1), Troubleshooting Guide (+3), License (+2), Contributing Guide (+3), TypeScript (+2), CI/CD Pipeline (+2), User Stories (+3), Functional Requirements (+2), Non-Functional Requirements (+3), Performance Metrics (+2), Future Considerations/Roadmap (+3), KPIs/Success Metrics (+3), Architecture/Flow Diagrams (+3), Code Quality Tools (Linting/Formatting) (+3)</t>
+          <t>E2E Tests (+1), Troubleshooting Guide (+1), Contributing Guide (+1), Docker Support (+1), Deployment Guide (+1), Kubernetes Support (+1), User Stories (+1), Non-Functional Requirements (+1), Future Considerations/Roadmap (+1), Architecture/Flow Diagrams (+1), Charts/Interactive Dashboards (+1), Code Quality Tools (Linting/Formatting) (+1), Accessibility Documentation (+1), Git Best Practices (Multiple Commits) (+1)</t>
         </is>
       </c>
     </row>
@@ -549,26 +549,26 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>38970</t>
+          <t>38981</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
-        <v>90.56047197640117</v>
+        <v>82.57374631268436</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>100</v>
+        <v>95.57374631268436</v>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>41/58</t>
+          <t>35/58</t>
         </is>
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
-          <t>E2E Tests (+3), Quick Start Guide (+1), Troubleshooting Guide (+3), License (+2), Contributing Guide (+3), TypeScript (+2), Docker Support (+3), CI/CD Pipeline (+2), Deployment Guide (+3), Kubernetes Support (+3), User Stories (+3), Functional Requirements (+2), Non-Functional Requirements (+3), Architecture Decision Records (ADRs) (+2), Performance Metrics (+2), Future Considerations/Roadmap (+3), Architecture/Flow Diagrams (+3), Charts/Interactive Dashboards (+3), Code Quality Tools (Linting/Formatting) (+3), Accessibility Documentation (+3), Git Best Practices (Multiple Commits) (+3)</t>
+          <t>Troubleshooting Guide (+1), Contributing Guide (+1), Export Functionality (+1), Docker Support (+1), GitHub Actions (+1), Deployment Guide (+1), Cost Analysis (+1), Architecture/Flow Diagrams (+1), Charts/Interactive Dashboards (+1), Code Quality Tools (Linting/Formatting) (+1), Plugin/Extension System (+1), Dual Interface (Multiple Frontends) (+1), Security Scanning (CodeQL) (+1)</t>
         </is>
       </c>
     </row>
@@ -578,17 +578,17 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>38981</t>
+          <t>38950</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>82.57374631268436</v>
+        <v>84.21091445427729</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>100</v>
+        <v>94.21091445427729</v>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
@@ -597,123 +597,123 @@
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t>Quick Start Guide (+1), Troubleshooting Guide (+3), License (+2), Contributing Guide (+3), Export Functionality (+3), Docker Support (+3), CI/CD Pipeline (+2), GitHub Actions (+3), Deployment Guide (+3), Cost Analysis (+3), Architecture/Flow Diagrams (+3), Charts/Interactive Dashboards (+3), Code Quality Tools (Linting/Formatting) (+3), Plugin/Extension System (+3), Dual Interface (Multiple Frontends) (+3), Security Scanning (CodeQL) (+3)</t>
+          <t>E2E Tests (+1), Integration Tests (+1), Troubleshooting Guide (+1), Contributing Guide (+1), User Stories (+1), Non-Functional Requirements (+1), Future Considerations/Roadmap (+1), KPIs/Success Metrics (+1), Architecture/Flow Diagrams (+1), Code Quality Tools (Linting/Formatting) (+1)</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>38959</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>75.81120943952801</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>79.81120943952801</v>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>26/58</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>Cost Analysis (+1), Parameter Investigation/Sensitivity Analysis (+1), Results Analysis Notebook (Jupyter) (+1), Architecture/Flow Diagrams (+1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>38960</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>75.81120943952801</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>79.81120943952801</v>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>26/58</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>Cost Analysis (+1), Parameter Investigation/Sensitivity Analysis (+1), Results Analysis Notebook (Jupyter) (+1), Architecture/Flow Diagrams (+1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="inlineStr">
         <is>
           <t>38951</t>
         </is>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C7" s="6" t="n">
         <v>76.62241887905606</v>
       </c>
-      <c r="D5" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>94.62241887905606</v>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
+      <c r="D7" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>79.62241887905606</v>
+      </c>
+      <c r="F7" s="5" t="inlineStr">
         <is>
           <t>26/58</t>
         </is>
       </c>
-      <c r="G5" s="4" t="inlineStr">
-        <is>
-          <t>Quick Start Guide (+1), Troubleshooting Guide (+3), License (+2), Contributing Guide (+3), TypeScript (+2), Docker Support (+3), CI/CD Pipeline (+2), Performance Metrics (+2)</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>38959</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>75.81120943952801</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3" t="n">
-        <v>92.81120943952801</v>
-      </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>26/58</t>
-        </is>
-      </c>
-      <c r="G6" s="4" t="inlineStr">
-        <is>
-          <t>Quick Start Guide (+1), Functional Requirements (+2), Architecture Decision Records (ADRs) (+2), Cost Analysis (+3), Parameter Investigation/Sensitivity Analysis (+3), Results Analysis Notebook (Jupyter) (+3), Architecture/Flow Diagrams (+3)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>38960</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>75.81120943952801</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3" t="n">
-        <v>92.81120943952801</v>
-      </c>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>26/58</t>
-        </is>
-      </c>
       <c r="G7" s="4" t="inlineStr">
         <is>
-          <t>Quick Start Guide (+1), Functional Requirements (+2), Architecture Decision Records (ADRs) (+2), Cost Analysis (+3), Parameter Investigation/Sensitivity Analysis (+3), Results Analysis Notebook (Jupyter) (+3), Architecture/Flow Diagrams (+3)</t>
+          <t>Troubleshooting Guide (+1), Contributing Guide (+1), Docker Support (+1)</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="inlineStr">
+      <c r="B8" s="5" t="inlineStr">
         <is>
           <t>38952</t>
         </is>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="6" t="n">
         <v>73.76106194690266</v>
       </c>
-      <c r="D8" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="E8" s="3" t="n">
-        <v>90.76106194690266</v>
-      </c>
-      <c r="F8" s="2" t="inlineStr">
+      <c r="D8" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>77.76106194690266</v>
+      </c>
+      <c r="F8" s="5" t="inlineStr">
         <is>
           <t>25/58</t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>Quick Start Guide (+1), Troubleshooting Guide (+3), License (+2), Contributing Guide (+3), Export Functionality (+3), User Profiles Feature (+3), Performance Metrics (+2)</t>
+          <t>Troubleshooting Guide (+1), Contributing Guide (+1), Export Functionality (+1), User Profiles Feature (+1)</t>
         </is>
       </c>
     </row>
@@ -730,10 +730,10 @@
         <v>65.7669616519174</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>79.7669616519174</v>
+        <v>69.7669616519174</v>
       </c>
       <c r="F9" s="5" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
       </c>
       <c r="G9" s="4" t="inlineStr">
         <is>
-          <t>Docker Support (+3), User Stories (+3), Functional Requirements (+2), Future Considerations/Roadmap (+3), Model Comparison Research (+3)</t>
+          <t>Docker Support (+1), User Stories (+1), Future Considerations/Roadmap (+1), Model Comparison Research (+1)</t>
         </is>
       </c>
     </row>
@@ -759,10 +759,10 @@
         <v>64.3362831858407</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>74.3362831858407</v>
+        <v>66.3362831858407</v>
       </c>
       <c r="F10" s="5" t="inlineStr">
         <is>
@@ -771,7 +771,7 @@
       </c>
       <c r="G10" s="4" t="inlineStr">
         <is>
-          <t>E2E Tests (+3), TypeScript (+2), Architecture Decision Records (ADRs) (+2), Code Quality Tools (Linting/Formatting) (+3)</t>
+          <t>E2E Tests (+1), Code Quality Tools (Linting/Formatting) (+1)</t>
         </is>
       </c>
     </row>
@@ -781,17 +781,17 @@
       </c>
       <c r="B11" s="5" t="inlineStr">
         <is>
-          <t>38988</t>
+          <t>59378</t>
         </is>
       </c>
       <c r="C11" s="6" t="n">
-        <v>59.61651917404129</v>
+        <v>59.62389380530973</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>72.61651917404129</v>
+        <v>62.62389380530973</v>
       </c>
       <c r="F11" s="5" t="inlineStr">
         <is>
@@ -800,7 +800,7 @@
       </c>
       <c r="G11" s="4" t="inlineStr">
         <is>
-          <t>TypeScript (+2), Docker Support (+3), CI/CD Pipeline (+2), GitHub Actions (+3), Model Comparison Research (+3)</t>
+          <t>GitHub Actions (+1), Dual Interface (Multiple Frontends) (+1), Security Scanning (CodeQL) (+1)</t>
         </is>
       </c>
     </row>
@@ -810,17 +810,17 @@
       </c>
       <c r="B12" s="5" t="inlineStr">
         <is>
-          <t>59378</t>
+          <t>38988</t>
         </is>
       </c>
       <c r="C12" s="6" t="n">
-        <v>59.62389380530973</v>
+        <v>59.61651917404129</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>70.62389380530973</v>
+        <v>62.61651917404129</v>
       </c>
       <c r="F12" s="5" t="inlineStr">
         <is>
@@ -829,7 +829,7 @@
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>CI/CD Pipeline (+2), GitHub Actions (+3), Dual Interface (Multiple Frontends) (+3), Security Scanning (CodeQL) (+3)</t>
+          <t>Docker Support (+1), GitHub Actions (+1), Model Comparison Research (+1)</t>
         </is>
       </c>
     </row>
@@ -839,17 +839,17 @@
       </c>
       <c r="B13" s="5" t="inlineStr">
         <is>
-          <t>38979</t>
+          <t>38993</t>
         </is>
       </c>
       <c r="C13" s="6" t="n">
-        <v>39.34365781710915</v>
+        <v>57.57374631268437</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>66.34365781710915</v>
+        <v>58.57374631268437</v>
       </c>
       <c r="F13" s="5" t="inlineStr">
         <is>
@@ -858,7 +858,7 @@
       </c>
       <c r="G13" s="4" t="inlineStr">
         <is>
-          <t>Deployment Guide (+3), User Stories (+3), Functional Requirements (+2), Architecture Decision Records (ADRs) (+2), Performance Metrics (+2), Cost Analysis (+3), KPIs/Success Metrics (+3), Model Comparison Research (+3), Accessibility Documentation (+3), Plugin/Extension System (+3)</t>
+          <t>Accessibility Documentation (+1)</t>
         </is>
       </c>
     </row>
@@ -868,26 +868,26 @@
       </c>
       <c r="B14" s="5" t="inlineStr">
         <is>
-          <t>38993</t>
+          <t>59375</t>
         </is>
       </c>
       <c r="C14" s="6" t="n">
-        <v>57.57374631268437</v>
+        <v>53.67256637168142</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>62.57374631268437</v>
+        <v>54.67256637168142</v>
       </c>
       <c r="F14" s="5" t="inlineStr">
         <is>
-          <t>16/58</t>
+          <t>14/58</t>
         </is>
       </c>
       <c r="G14" s="4" t="inlineStr">
         <is>
-          <t>TypeScript (+2), Accessibility Documentation (+3)</t>
+          <t>Parameter Investigation/Sensitivity Analysis (+1)</t>
         </is>
       </c>
     </row>
@@ -897,26 +897,26 @@
       </c>
       <c r="B15" s="5" t="inlineStr">
         <is>
-          <t>59375</t>
+          <t>59373</t>
         </is>
       </c>
       <c r="C15" s="6" t="n">
-        <v>53.67256637168142</v>
+        <v>48.96755162241888</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>57.67256637168142</v>
+        <v>50.96755162241888</v>
       </c>
       <c r="F15" s="5" t="inlineStr">
         <is>
-          <t>14/58</t>
+          <t>15/58</t>
         </is>
       </c>
       <c r="G15" s="4" t="inlineStr">
         <is>
-          <t>Quick Start Guide (+1), Parameter Investigation/Sensitivity Analysis (+3)</t>
+          <t>Export Functionality (+1), User Profiles Feature (+1)</t>
         </is>
       </c>
     </row>
@@ -926,26 +926,26 @@
       </c>
       <c r="B16" s="5" t="inlineStr">
         <is>
-          <t>59373</t>
+          <t>38963</t>
         </is>
       </c>
       <c r="C16" s="6" t="n">
-        <v>48.96755162241888</v>
+        <v>49.99262536873157</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>56.96755162241888</v>
+        <v>49.99262536873157</v>
       </c>
       <c r="F16" s="5" t="inlineStr">
         <is>
-          <t>15/58</t>
+          <t>13/58</t>
         </is>
       </c>
       <c r="G16" s="4" t="inlineStr">
         <is>
-          <t>License (+2), Export Functionality (+3), User Profiles Feature (+3)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -955,26 +955,26 @@
       </c>
       <c r="B17" s="5" t="inlineStr">
         <is>
-          <t>38980</t>
+          <t>38979</t>
         </is>
       </c>
       <c r="C17" s="6" t="n">
-        <v>36.6740412979351</v>
+        <v>39.34365781710915</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>55.6740412979351</v>
+        <v>46.34365781710915</v>
       </c>
       <c r="F17" s="5" t="inlineStr">
         <is>
-          <t>13/58</t>
+          <t>16/58</t>
         </is>
       </c>
       <c r="G17" s="4" t="inlineStr">
         <is>
-          <t>Deployment Guide (+3), Architecture Decision Records (ADRs) (+2), Performance Metrics (+2), Cost Analysis (+3), Model Comparison Research (+3), Accessibility Documentation (+3), Voice Input Support (+3)</t>
+          <t>Deployment Guide (+1), User Stories (+1), Cost Analysis (+1), KPIs/Success Metrics (+1), Model Comparison Research (+1), Accessibility Documentation (+1), Plugin/Extension System (+1)</t>
         </is>
       </c>
     </row>
@@ -984,17 +984,17 @@
       </c>
       <c r="B18" s="5" t="inlineStr">
         <is>
-          <t>38963</t>
+          <t>38980</t>
         </is>
       </c>
       <c r="C18" s="6" t="n">
-        <v>49.99262536873157</v>
+        <v>36.6740412979351</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>49.99262536873157</v>
+        <v>41.6740412979351</v>
       </c>
       <c r="F18" s="5" t="inlineStr">
         <is>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="G18" s="4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Deployment Guide (+1), Cost Analysis (+1), Model Comparison Research (+1), Accessibility Documentation (+1), Voice Input Support (+1)</t>
         </is>
       </c>
     </row>
@@ -1013,26 +1013,26 @@
       </c>
       <c r="B19" s="5" t="inlineStr">
         <is>
-          <t>38989</t>
+          <t>38962</t>
         </is>
       </c>
       <c r="C19" s="6" t="n">
-        <v>34.41002949852508</v>
+        <v>37.69911504424779</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>38.41002949852508</v>
+        <v>37.69911504424779</v>
       </c>
       <c r="F19" s="5" t="inlineStr">
         <is>
-          <t>9/58</t>
+          <t>8/58</t>
         </is>
       </c>
       <c r="G19" s="4" t="inlineStr">
         <is>
-          <t>TypeScript (+2), CI/CD Pipeline (+2)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1042,17 +1042,17 @@
       </c>
       <c r="B20" s="5" t="inlineStr">
         <is>
-          <t>38962</t>
+          <t>38954</t>
         </is>
       </c>
       <c r="C20" s="6" t="n">
-        <v>37.69911504424779</v>
+        <v>36.46755162241888</v>
       </c>
       <c r="D20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>37.69911504424779</v>
+        <v>36.46755162241888</v>
       </c>
       <c r="F20" s="5" t="inlineStr">
         <is>
@@ -1071,21 +1071,21 @@
       </c>
       <c r="B21" s="5" t="inlineStr">
         <is>
-          <t>38954</t>
+          <t>38989</t>
         </is>
       </c>
       <c r="C21" s="6" t="n">
-        <v>36.46755162241888</v>
+        <v>34.41002949852508</v>
       </c>
       <c r="D21" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>36.46755162241888</v>
+        <v>34.41002949852508</v>
       </c>
       <c r="F21" s="5" t="inlineStr">
         <is>
-          <t>8/58</t>
+          <t>9/58</t>
         </is>
       </c>
       <c r="G21" s="4" t="inlineStr">
@@ -1129,26 +1129,26 @@
       </c>
       <c r="B23" s="5" t="inlineStr">
         <is>
-          <t>59376</t>
+          <t>38955</t>
         </is>
       </c>
       <c r="C23" s="6" t="n">
-        <v>30.12536873156342</v>
+        <v>32.98672566371681</v>
       </c>
       <c r="D23" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>33.12536873156342</v>
+        <v>32.98672566371681</v>
       </c>
       <c r="F23" s="5" t="inlineStr">
         <is>
-          <t>8/58</t>
+          <t>7/58</t>
         </is>
       </c>
       <c r="G23" s="4" t="inlineStr">
         <is>
-          <t>File Upload Support (+3)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1158,17 +1158,17 @@
       </c>
       <c r="B24" s="5" t="inlineStr">
         <is>
-          <t>38955</t>
+          <t>38990</t>
         </is>
       </c>
       <c r="C24" s="6" t="n">
-        <v>32.98672566371681</v>
+        <v>31.96165191740413</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>32.98672566371681</v>
+        <v>31.96165191740413</v>
       </c>
       <c r="F24" s="5" t="inlineStr">
         <is>
@@ -1187,26 +1187,26 @@
       </c>
       <c r="B25" s="5" t="inlineStr">
         <is>
-          <t>38990</t>
+          <t>59376</t>
         </is>
       </c>
       <c r="C25" s="6" t="n">
-        <v>31.96165191740413</v>
+        <v>30.12536873156342</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>31.96165191740413</v>
+        <v>31.12536873156342</v>
       </c>
       <c r="F25" s="5" t="inlineStr">
         <is>
-          <t>7/58</t>
+          <t>8/58</t>
         </is>
       </c>
       <c r="G25" s="4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>File Upload Support (+1)</t>
         </is>
       </c>
     </row>
@@ -1274,26 +1274,26 @@
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
-          <t>38957</t>
+          <t>38966</t>
         </is>
       </c>
       <c r="C28" s="6" t="n">
-        <v>23.55457227138643</v>
+        <v>24.58702064896755</v>
       </c>
       <c r="D28" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>26.55457227138643</v>
+        <v>24.58702064896755</v>
       </c>
       <c r="F28" s="5" t="inlineStr">
         <is>
-          <t>5/58</t>
+          <t>4/58</t>
         </is>
       </c>
       <c r="G28" s="4" t="inlineStr">
         <is>
-          <t>Git Best Practices (Multiple Commits) (+3)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1303,17 +1303,17 @@
       </c>
       <c r="B29" s="5" t="inlineStr">
         <is>
-          <t>38971</t>
+          <t>38957</t>
         </is>
       </c>
       <c r="C29" s="6" t="n">
         <v>23.55457227138643</v>
       </c>
       <c r="D29" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E29" s="6" t="n">
-        <v>26.55457227138643</v>
+        <v>24.55457227138643</v>
       </c>
       <c r="F29" s="5" t="inlineStr">
         <is>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="G29" s="4" t="inlineStr">
         <is>
-          <t>Multi-Agent Orchestration (+3)</t>
+          <t>Git Best Practices (Multiple Commits) (+1)</t>
         </is>
       </c>
     </row>
@@ -1332,17 +1332,17 @@
       </c>
       <c r="B30" s="5" t="inlineStr">
         <is>
-          <t>38973</t>
+          <t>38971</t>
         </is>
       </c>
       <c r="C30" s="6" t="n">
-        <v>21.92477876106195</v>
+        <v>23.55457227138643</v>
       </c>
       <c r="D30" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E30" s="6" t="n">
-        <v>24.92477876106195</v>
+        <v>24.55457227138643</v>
       </c>
       <c r="F30" s="5" t="inlineStr">
         <is>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="G30" s="4" t="inlineStr">
         <is>
-          <t>Multi-Agent Orchestration (+3)</t>
+          <t>Multi-Agent Orchestration (+1)</t>
         </is>
       </c>
     </row>
@@ -1361,26 +1361,26 @@
       </c>
       <c r="B31" s="5" t="inlineStr">
         <is>
-          <t>38966</t>
+          <t>38973</t>
         </is>
       </c>
       <c r="C31" s="6" t="n">
-        <v>24.58702064896755</v>
+        <v>21.92477876106195</v>
       </c>
       <c r="D31" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="6" t="n">
-        <v>24.58702064896755</v>
+        <v>22.92477876106195</v>
       </c>
       <c r="F31" s="5" t="inlineStr">
         <is>
-          <t>4/58</t>
+          <t>5/58</t>
         </is>
       </c>
       <c r="G31" s="4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Multi-Agent Orchestration (+1)</t>
         </is>
       </c>
     </row>
@@ -1390,17 +1390,17 @@
       </c>
       <c r="B32" s="5" t="inlineStr">
         <is>
-          <t>38961</t>
+          <t>38958</t>
         </is>
       </c>
       <c r="C32" s="6" t="n">
-        <v>19.25516224188791</v>
+        <v>20.48672566371681</v>
       </c>
       <c r="D32" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E32" s="6" t="n">
-        <v>22.25516224188791</v>
+        <v>20.48672566371681</v>
       </c>
       <c r="F32" s="5" t="inlineStr">
         <is>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="G32" s="4" t="inlineStr">
         <is>
-          <t>Git Best Practices (Multiple Commits) (+3)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="B33" s="5" t="inlineStr">
         <is>
-          <t>38958</t>
+          <t>38964</t>
         </is>
       </c>
       <c r="C33" s="6" t="n">
@@ -1448,17 +1448,17 @@
       </c>
       <c r="B34" s="5" t="inlineStr">
         <is>
-          <t>38964</t>
+          <t>38961</t>
         </is>
       </c>
       <c r="C34" s="6" t="n">
-        <v>20.48672566371681</v>
+        <v>19.25516224188791</v>
       </c>
       <c r="D34" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="6" t="n">
-        <v>20.48672566371681</v>
+        <v>20.25516224188791</v>
       </c>
       <c r="F34" s="5" t="inlineStr">
         <is>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="G34" s="4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Git Best Practices (Multiple Commits) (+1)</t>
         </is>
       </c>
     </row>
@@ -1506,26 +1506,26 @@
       </c>
       <c r="B36" s="5" t="inlineStr">
         <is>
-          <t>38985</t>
+          <t>38986</t>
         </is>
       </c>
       <c r="C36" s="6" t="n">
-        <v>8.399705014749262</v>
+        <v>13.31858407079646</v>
       </c>
       <c r="D36" s="5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E36" s="6" t="n">
-        <v>14.39970501474926</v>
+        <v>13.31858407079646</v>
       </c>
       <c r="F36" s="5" t="inlineStr">
         <is>
-          <t>3/58</t>
+          <t>2/58</t>
         </is>
       </c>
       <c r="G36" s="4" t="inlineStr">
         <is>
-          <t>Integration Tests (+3), Multi-Agent Orchestration (+3)</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1535,26 +1535,26 @@
       </c>
       <c r="B37" s="5" t="inlineStr">
         <is>
-          <t>38986</t>
+          <t>38985</t>
         </is>
       </c>
       <c r="C37" s="6" t="n">
-        <v>13.31858407079646</v>
+        <v>8.399705014749262</v>
       </c>
       <c r="D37" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E37" s="6" t="n">
-        <v>13.31858407079646</v>
+        <v>10.39970501474926</v>
       </c>
       <c r="F37" s="5" t="inlineStr">
         <is>
-          <t>2/58</t>
+          <t>3/58</t>
         </is>
       </c>
       <c r="G37" s="4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Integration Tests (+1), Multi-Agent Orchestration (+1)</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="C2" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D2" s="8" t="inlineStr">
@@ -1640,7 +1640,7 @@
       </c>
       <c r="C3" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D3" s="8" t="inlineStr">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="C4" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D4" s="8" t="inlineStr">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="C5" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D5" s="8" t="inlineStr">
@@ -1706,7 +1706,7 @@
       </c>
       <c r="C6" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D6" s="8" t="inlineStr">
@@ -1728,7 +1728,7 @@
       </c>
       <c r="C7" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D7" s="8" t="inlineStr">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="C8" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D8" s="8" t="inlineStr">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C9" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D9" s="8" t="inlineStr">
@@ -1794,7 +1794,7 @@
       </c>
       <c r="C10" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D10" s="8" t="inlineStr">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="C11" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D11" s="8" t="inlineStr">
@@ -1838,7 +1838,7 @@
       </c>
       <c r="C12" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D12" s="8" t="inlineStr">
@@ -1860,7 +1860,7 @@
       </c>
       <c r="C13" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D13" s="8" t="inlineStr">
@@ -1882,7 +1882,7 @@
       </c>
       <c r="C14" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D14" s="8" t="inlineStr">
@@ -1904,7 +1904,7 @@
       </c>
       <c r="C15" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D15" s="8" t="inlineStr">
@@ -1926,7 +1926,7 @@
       </c>
       <c r="C16" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D16" s="8" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="C17" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D17" s="8" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="C18" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D18" s="8" t="inlineStr">
@@ -1992,7 +1992,7 @@
       </c>
       <c r="C19" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D19" s="8" t="inlineStr">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="C20" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D20" s="8" t="inlineStr">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="C21" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D21" s="8" t="inlineStr">
@@ -2058,7 +2058,7 @@
       </c>
       <c r="C22" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D22" s="8" t="inlineStr">
@@ -2080,7 +2080,7 @@
       </c>
       <c r="C23" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D23" s="8" t="inlineStr">
@@ -2102,7 +2102,7 @@
       </c>
       <c r="C24" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D24" s="8" t="inlineStr">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="C25" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D25" s="8" t="inlineStr">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="C26" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="C27" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D27" s="8" t="inlineStr">
@@ -2190,7 +2190,7 @@
       </c>
       <c r="C28" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D28" s="8" t="inlineStr">
@@ -2212,7 +2212,7 @@
       </c>
       <c r="C29" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D29" s="8" t="inlineStr">
@@ -2234,166 +2234,12 @@
       </c>
       <c r="C30" s="8" t="inlineStr">
         <is>
-          <t>+3</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
           <t>38950, 38959, 38960, 38970, 38981</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="8" t="inlineStr">
-        <is>
-          <t>License</t>
-        </is>
-      </c>
-      <c r="B31" s="8" t="inlineStr">
-        <is>
-          <t>16.7%</t>
-        </is>
-      </c>
-      <c r="C31" s="8" t="inlineStr">
-        <is>
-          <t>+2</t>
-        </is>
-      </c>
-      <c r="D31" s="8" t="inlineStr">
-        <is>
-          <t>38950, 38951, 38952, 38970, 38981, 59373</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="8" t="inlineStr">
-        <is>
-          <t>Functional Requirements</t>
-        </is>
-      </c>
-      <c r="B32" s="8" t="inlineStr">
-        <is>
-          <t>16.7%</t>
-        </is>
-      </c>
-      <c r="C32" s="8" t="inlineStr">
-        <is>
-          <t>+2</t>
-        </is>
-      </c>
-      <c r="D32" s="8" t="inlineStr">
-        <is>
-          <t>38950, 38953, 38959, 38960, 38970, 38979</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="8" t="inlineStr">
-        <is>
-          <t>Architecture Decision Records (ADRs)</t>
-        </is>
-      </c>
-      <c r="B33" s="8" t="inlineStr">
-        <is>
-          <t>16.7%</t>
-        </is>
-      </c>
-      <c r="C33" s="8" t="inlineStr">
-        <is>
-          <t>+2</t>
-        </is>
-      </c>
-      <c r="D33" s="8" t="inlineStr">
-        <is>
-          <t>38959, 38960, 38970, 38979, 38980, 38982</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="8" t="inlineStr">
-        <is>
-          <t>Performance Metrics</t>
-        </is>
-      </c>
-      <c r="B34" s="8" t="inlineStr">
-        <is>
-          <t>16.7%</t>
-        </is>
-      </c>
-      <c r="C34" s="8" t="inlineStr">
-        <is>
-          <t>+2</t>
-        </is>
-      </c>
-      <c r="D34" s="8" t="inlineStr">
-        <is>
-          <t>38950, 38951, 38952, 38970, 38979, 38980</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="8" t="inlineStr">
-        <is>
-          <t>TypeScript</t>
-        </is>
-      </c>
-      <c r="B35" s="8" t="inlineStr">
-        <is>
-          <t>19.4%</t>
-        </is>
-      </c>
-      <c r="C35" s="8" t="inlineStr">
-        <is>
-          <t>+2</t>
-        </is>
-      </c>
-      <c r="D35" s="8" t="inlineStr">
-        <is>
-          <t>38950, 38951, 38970, 38982, 38988, 38989, 38993</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="8" t="inlineStr">
-        <is>
-          <t>CI/CD Pipeline</t>
-        </is>
-      </c>
-      <c r="B36" s="8" t="inlineStr">
-        <is>
-          <t>19.4%</t>
-        </is>
-      </c>
-      <c r="C36" s="8" t="inlineStr">
-        <is>
-          <t>+2</t>
-        </is>
-      </c>
-      <c r="D36" s="8" t="inlineStr">
-        <is>
-          <t>38950, 38951, 38970, 38981, 38988, 38989, 59378</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="8" t="inlineStr">
-        <is>
-          <t>Quick Start Guide</t>
-        </is>
-      </c>
-      <c r="B37" s="8" t="inlineStr">
-        <is>
-          <t>22.2%</t>
-        </is>
-      </c>
-      <c r="C37" s="8" t="inlineStr">
-        <is>
-          <t>+1</t>
-        </is>
-      </c>
-      <c r="D37" s="8" t="inlineStr">
-        <is>
-          <t>38950, 38951, 38952, 38959, 38960, 38970, 38981, 59375</t>
         </is>
       </c>
     </row>

</xml_diff>